<commit_message>
DEMOGRAPHY: Get Marital Status data
</commit_message>
<xml_diff>
--- a/files/demographic/maritalStatus/estado-civil.xlsx
+++ b/files/demographic/maritalStatus/estado-civil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arlindo Boa\Desktop\tactic\files\demographic\maritalStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59FADAA-CC75-4C8A-B30D-A74050F80B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E187E17-CF00-4022-B20D-ADAF191D3C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="629">
   <si>
     <t>Sexo</t>
   </si>
@@ -1919,6 +1919,9 @@
   <si>
     <t>Desconhecido</t>
   </si>
+  <si>
+    <t>#</t>
+  </si>
 </sst>
 </file>
 
@@ -1956,10 +1959,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -45063,8 +45067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H179" sqref="H179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49498,6 +49502,9 @@
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>628</v>
+      </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -52434,6 +52441,9 @@
       </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>628</v>
+      </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -55251,6 +55261,9 @@
       </c>
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>628</v>
+      </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -58782,6 +58795,9 @@
       </c>
     </row>
     <row r="121" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>628</v>
+      </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -60528,6 +60544,9 @@
       </c>
     </row>
     <row r="136" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>628</v>
+      </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -62274,6 +62293,9 @@
       </c>
     </row>
     <row r="151" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>628</v>
+      </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -64139,6 +64161,9 @@
       </c>
     </row>
     <row r="167" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>628</v>
+      </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -65549,7 +65574,7 @@
       <c r="G179" s="1">
         <v>4343</v>
       </c>
-      <c r="H179" s="1">
+      <c r="H179" s="3">
         <v>45801</v>
       </c>
       <c r="I179" s="1">
@@ -66243,5 +66268,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>